<commit_message>
import change to merge benchmarks
</commit_message>
<xml_diff>
--- a/data/imports/vbc-import-final.xlsx
+++ b/data/imports/vbc-import-final.xlsx
@@ -175,12 +175,6 @@
     <t>population</t>
   </si>
   <si>
-    <t>median_household_inc</t>
-  </si>
-  <si>
-    <t>poverty_rate</t>
-  </si>
-  <si>
     <t>fireresponse</t>
   </si>
   <si>
@@ -269,6 +263,12 @@
   </si>
   <si>
     <t>A+</t>
+  </si>
+  <si>
+    <t>median_household_income</t>
+  </si>
+  <si>
+    <t>poverty</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
   <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,102 +734,102 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.2">
@@ -1173,7 +1173,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="13">
-        <v>100003</v>
+        <v>100004</v>
       </c>
       <c r="C7" s="3">
         <v>72275</v>
@@ -1782,7 +1782,7 @@
   <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1882,102 +1882,102 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.2">
@@ -2321,7 +2321,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="13">
-        <v>100003</v>
+        <v>100004</v>
       </c>
       <c r="C7" s="3">
         <v>74743</v>
@@ -2934,7 +2934,7 @@
   <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3034,102 +3034,102 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.2">
@@ -3423,7 +3423,7 @@
         <v>5.44</v>
       </c>
       <c r="AF5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="18" x14ac:dyDescent="0.2">
@@ -3521,7 +3521,7 @@
         <v>7.3289080147903229</v>
       </c>
       <c r="AF6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="18" x14ac:dyDescent="0.2">
@@ -3529,7 +3529,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="13">
-        <v>100003</v>
+        <v>100004</v>
       </c>
       <c r="C7" s="3">
         <v>78189</v>

</xml_diff>

<commit_message>
fix time formats in vbc import file
</commit_message>
<xml_diff>
--- a/data/imports/vbc-import-final.xlsx
+++ b/data/imports/vbc-import-final.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfergu15/Documents/envisio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/envisio/data/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="-19540" windowWidth="27360" windowHeight="15120" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="7860" yWindow="-19540" windowWidth="27360" windowHeight="15120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="2014" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="137">
   <si>
     <t>Benchmark</t>
   </si>
@@ -269,20 +269,187 @@
   </si>
   <si>
     <t>poverty</t>
+  </si>
+  <si>
+    <t>3:30</t>
+  </si>
+  <si>
+    <t>6:09</t>
+  </si>
+  <si>
+    <t>4:11</t>
+  </si>
+  <si>
+    <t>6:07</t>
+  </si>
+  <si>
+    <t>3:15</t>
+  </si>
+  <si>
+    <t>3:54</t>
+  </si>
+  <si>
+    <t>7:01</t>
+  </si>
+  <si>
+    <t>6:12</t>
+  </si>
+  <si>
+    <t>5:11</t>
+  </si>
+  <si>
+    <t>5:03</t>
+  </si>
+  <si>
+    <t>6:31</t>
+  </si>
+  <si>
+    <t>3:48</t>
+  </si>
+  <si>
+    <t>5:18</t>
+  </si>
+  <si>
+    <t>5:01</t>
+  </si>
+  <si>
+    <t>6:27</t>
+  </si>
+  <si>
+    <t>5:46</t>
+  </si>
+  <si>
+    <t>4:29</t>
+  </si>
+  <si>
+    <t>4:32</t>
+  </si>
+  <si>
+    <t>5:50</t>
+  </si>
+  <si>
+    <t>4:16</t>
+  </si>
+  <si>
+    <t>6:14</t>
+  </si>
+  <si>
+    <t>3:58</t>
+  </si>
+  <si>
+    <t>4:59</t>
+  </si>
+  <si>
+    <t>4:44</t>
+  </si>
+  <si>
+    <t>5:05</t>
+  </si>
+  <si>
+    <t>5:34</t>
+  </si>
+  <si>
+    <t>4:48</t>
+  </si>
+  <si>
+    <t>5:25</t>
+  </si>
+  <si>
+    <t>5:28</t>
+  </si>
+  <si>
+    <t>4:13</t>
+  </si>
+  <si>
+    <t>4:23</t>
+  </si>
+  <si>
+    <t>6:21</t>
+  </si>
+  <si>
+    <t>4:53</t>
+  </si>
+  <si>
+    <t>5:09</t>
+  </si>
+  <si>
+    <t>4:00</t>
+  </si>
+  <si>
+    <t>6:41</t>
+  </si>
+  <si>
+    <t>5:12</t>
+  </si>
+  <si>
+    <t>4:36</t>
+  </si>
+  <si>
+    <t>6:36</t>
+  </si>
+  <si>
+    <t>7:18</t>
+  </si>
+  <si>
+    <t>4:57</t>
+  </si>
+  <si>
+    <t>4:30</t>
+  </si>
+  <si>
+    <t>5:52</t>
+  </si>
+  <si>
+    <t>5:56</t>
+  </si>
+  <si>
+    <t>5:26</t>
+  </si>
+  <si>
+    <t>5:47</t>
+  </si>
+  <si>
+    <t>4:07</t>
+  </si>
+  <si>
+    <t>7:34</t>
+  </si>
+  <si>
+    <t>6:15</t>
+  </si>
+  <si>
+    <t>4:18</t>
+  </si>
+  <si>
+    <t>4:42</t>
+  </si>
+  <si>
+    <t>4:05</t>
+  </si>
+  <si>
+    <t>4:49</t>
+  </si>
+  <si>
+    <t>6:26</t>
+  </si>
+  <si>
+    <t>5:32</t>
+  </si>
+  <si>
+    <t>6:23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="169" formatCode="h:mm;@"/>
-    <numFmt numFmtId="170" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -342,17 +509,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -633,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,7 +911,7 @@
       <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>79</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -836,7 +1003,7 @@
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>100000</v>
       </c>
       <c r="C3" s="3">
@@ -848,68 +1015,68 @@
       <c r="E3" s="5">
         <v>0.19089999999999999</v>
       </c>
-      <c r="F3" s="6">
-        <v>0.30416666666666664</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="F3" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="6">
         <v>8.4599999999999995E-2</v>
       </c>
-      <c r="H3" s="6">
-        <v>0.31527777777777777</v>
-      </c>
-      <c r="I3" s="7">
+      <c r="H3" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="I3" s="6">
         <v>0.69</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6">
         <v>2.6</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="6">
         <v>47.2</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="7">
         <v>0.53700000000000003</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="7">
         <v>0.224</v>
       </c>
       <c r="P3">
         <v>2</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="Q3" s="8">
         <v>52.21</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3" s="6">
         <v>2.21</v>
       </c>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="7">
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="6">
         <v>0</v>
       </c>
-      <c r="W3" s="10">
+      <c r="W3" s="9">
         <v>57.16</v>
       </c>
-      <c r="X3" s="10">
+      <c r="X3" s="9">
         <v>44.29</v>
       </c>
-      <c r="Y3" s="10">
+      <c r="Y3" s="9">
         <v>22.18</v>
       </c>
-      <c r="Z3" s="10">
+      <c r="Z3" s="9">
         <v>31.61</v>
       </c>
-      <c r="AA3" s="10">
+      <c r="AA3" s="9">
         <v>20</v>
       </c>
-      <c r="AB3" s="11">
+      <c r="AB3" s="10">
         <v>0.18</v>
       </c>
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
-      <c r="AE3" s="12">
+      <c r="AE3" s="11">
         <v>6.4</v>
       </c>
       <c r="AF3" t="s">
@@ -920,7 +1087,7 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>100001</v>
       </c>
       <c r="C4" s="3">
@@ -932,68 +1099,68 @@
       <c r="E4" s="5">
         <v>0.1041</v>
       </c>
-      <c r="F4" s="6">
-        <v>0.16527777777777777</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="F4" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="6">
         <v>8.3900000000000002E-2</v>
       </c>
-      <c r="H4" s="6">
-        <v>0.26041666666666669</v>
-      </c>
-      <c r="I4" s="7">
+      <c r="H4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4" s="6">
         <v>0.59</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6">
         <v>2.34</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="6">
         <v>23.96</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="7">
         <v>0.42099999999999999</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="7">
         <v>0.17199999999999999</v>
       </c>
       <c r="P4">
         <v>4</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="8">
         <v>58.53</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="6">
         <v>3.63</v>
       </c>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="7">
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="6">
         <v>0.03</v>
       </c>
-      <c r="W4" s="10">
+      <c r="W4" s="9">
         <v>57.16</v>
       </c>
-      <c r="X4" s="10">
+      <c r="X4" s="9">
         <v>26.35</v>
       </c>
-      <c r="Y4" s="10">
+      <c r="Y4" s="9">
         <v>24.51</v>
       </c>
-      <c r="Z4" s="10">
+      <c r="Z4" s="9">
         <v>26.35</v>
       </c>
-      <c r="AA4" s="10">
+      <c r="AA4" s="9">
         <v>15.07</v>
       </c>
-      <c r="AB4" s="11">
+      <c r="AB4" s="10">
         <v>0.18</v>
       </c>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
-      <c r="AE4" s="12">
+      <c r="AE4" s="11">
         <v>6.48</v>
       </c>
       <c r="AF4" t="s">
@@ -1004,7 +1171,7 @@
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>100002</v>
       </c>
       <c r="C5" s="3">
@@ -1016,68 +1183,68 @@
       <c r="E5" s="5">
         <v>5.91E-2</v>
       </c>
-      <c r="F5" s="6">
-        <v>0.20625000000000002</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="F5" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="6">
         <v>6.88E-2</v>
       </c>
-      <c r="H5" s="6">
-        <v>0.17916666666666667</v>
-      </c>
-      <c r="I5" s="7">
+      <c r="H5" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" s="6">
         <v>0.27</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7">
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6">
         <v>0.85</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="6">
         <v>15.25</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="7">
         <v>0.69199999999999995</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="7">
         <v>0.22</v>
       </c>
       <c r="P5">
         <v>2</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="Q5" s="8">
         <v>55</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="6">
         <v>2.63</v>
       </c>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="7">
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="6">
         <v>0.17100000000000001</v>
       </c>
-      <c r="W5" s="10">
+      <c r="W5" s="9">
         <v>40.67</v>
       </c>
-      <c r="X5" s="10">
+      <c r="X5" s="9">
         <v>30.78</v>
       </c>
-      <c r="Y5" s="10">
+      <c r="Y5" s="9">
         <v>24.35</v>
       </c>
-      <c r="Z5" s="10">
+      <c r="Z5" s="9">
         <v>25.82</v>
       </c>
-      <c r="AA5" s="10">
+      <c r="AA5" s="9">
         <v>16.399999999999999</v>
       </c>
-      <c r="AB5" s="11">
+      <c r="AB5" s="10">
         <v>0.17</v>
       </c>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
-      <c r="AE5" s="12">
+      <c r="AE5" s="11">
         <v>5.44</v>
       </c>
       <c r="AF5" t="s">
@@ -1088,7 +1255,7 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>100003</v>
       </c>
       <c r="C6" s="3">
@@ -1100,68 +1267,68 @@
       <c r="E6" s="5">
         <v>0.26300000000000001</v>
       </c>
-      <c r="F6" s="6">
-        <v>0.1875</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="F6" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="6">
         <v>0.16889999999999999</v>
       </c>
-      <c r="H6" s="6">
-        <v>0.19583333333333333</v>
-      </c>
-      <c r="I6" s="7">
+      <c r="H6" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="I6" s="6">
         <v>0.6</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7">
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6">
         <v>3.92</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="6">
         <v>58.96</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="7">
         <v>0.38</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <v>0.06</v>
       </c>
       <c r="P6">
         <v>3</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="Q6" s="8">
         <v>35.18</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="6">
         <v>8.43</v>
       </c>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="7">
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="6">
         <v>0.19900000000000001</v>
       </c>
-      <c r="W6" s="10">
+      <c r="W6" s="9">
         <v>61.88</v>
       </c>
-      <c r="X6" s="10">
+      <c r="X6" s="9">
         <v>51.92</v>
       </c>
-      <c r="Y6" s="10">
+      <c r="Y6" s="9">
         <v>33.18</v>
       </c>
-      <c r="Z6" s="10">
+      <c r="Z6" s="9">
         <v>37.68</v>
       </c>
-      <c r="AA6" s="10">
+      <c r="AA6" s="9">
         <v>16.3</v>
       </c>
-      <c r="AB6" s="11">
+      <c r="AB6" s="10">
         <v>0.16</v>
       </c>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="12">
+      <c r="AE6" s="11">
         <v>6.89</v>
       </c>
       <c r="AF6" t="s">
@@ -1172,7 +1339,7 @@
       <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>100004</v>
       </c>
       <c r="C7" s="3">
@@ -1184,68 +1351,68 @@
       <c r="E7" s="5">
         <v>0.10780000000000001</v>
       </c>
-      <c r="F7" s="6">
-        <v>0.24444444444444446</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="F7" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="6">
         <v>6.9900000000000004E-2</v>
       </c>
-      <c r="H7" s="6">
-        <v>0.17013888888888887</v>
-      </c>
-      <c r="I7" s="7">
+      <c r="H7" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="I7" s="6">
         <v>0.31</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7">
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6">
         <v>1.3</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <v>23.74</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="7">
         <v>0.48799999999999999</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="7">
         <v>0.20899999999999999</v>
       </c>
       <c r="P7">
         <v>1</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="8">
         <v>48</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="6">
         <v>4.67</v>
       </c>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="7">
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="6">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="W7" s="10">
+      <c r="W7" s="9">
         <v>70.34</v>
       </c>
-      <c r="X7" s="10">
+      <c r="X7" s="9">
         <v>104.78</v>
       </c>
-      <c r="Y7" s="10">
+      <c r="Y7" s="9">
         <v>32.5</v>
       </c>
-      <c r="Z7" s="10">
+      <c r="Z7" s="9">
         <v>69.349999999999994</v>
       </c>
-      <c r="AA7" s="10">
+      <c r="AA7" s="9">
         <v>22.8</v>
       </c>
-      <c r="AB7" s="11">
+      <c r="AB7" s="10">
         <v>0.25</v>
       </c>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
-      <c r="AE7" s="12">
+      <c r="AE7" s="11">
         <v>7.07</v>
       </c>
       <c r="AF7" t="s">
@@ -1256,7 +1423,7 @@
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>100005</v>
       </c>
       <c r="C8" s="3">
@@ -1268,68 +1435,68 @@
       <c r="E8" s="5">
         <v>0.16639999999999999</v>
       </c>
-      <c r="F8" s="6">
-        <v>0.20902777777777778</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="F8" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="6">
         <v>0.12770000000000001</v>
       </c>
-      <c r="H8" s="6">
-        <v>0.20069444444444443</v>
-      </c>
-      <c r="I8" s="7">
+      <c r="H8" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I8" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7">
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6">
         <v>4.01</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <v>28.68</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="7">
         <v>0.47599999999999998</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="7">
         <v>0.29499999999999998</v>
       </c>
       <c r="P8">
         <v>4</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="Q8" s="8">
         <v>57.94</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="6">
         <v>2.74</v>
       </c>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="7">
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="6">
         <v>0.12</v>
       </c>
-      <c r="W8" s="10">
+      <c r="W8" s="9">
         <v>77.650000000000006</v>
       </c>
-      <c r="X8" s="10">
+      <c r="X8" s="9">
         <v>49.17</v>
       </c>
-      <c r="Y8" s="10">
+      <c r="Y8" s="9">
         <v>46.63</v>
       </c>
-      <c r="Z8" s="10">
+      <c r="Z8" s="9">
         <v>43.53</v>
       </c>
-      <c r="AA8" s="10">
+      <c r="AA8" s="9">
         <v>26.09</v>
       </c>
-      <c r="AB8" s="11">
+      <c r="AB8" s="10">
         <v>0.23</v>
       </c>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
-      <c r="AE8" s="12">
+      <c r="AE8" s="11">
         <v>8.24</v>
       </c>
       <c r="AF8" t="s">
@@ -1340,7 +1507,7 @@
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>100006</v>
       </c>
       <c r="C9" s="3">
@@ -1352,63 +1519,63 @@
       <c r="E9" s="5">
         <v>0.11509999999999999</v>
       </c>
-      <c r="F9" s="6">
-        <v>0.24722222222222223</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="F9" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" s="6">
         <v>9.2200000000000004E-2</v>
       </c>
-      <c r="H9" s="6">
-        <v>0.26805555555555555</v>
-      </c>
-      <c r="I9" s="7">
+      <c r="H9" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="I9" s="6">
         <v>0.33</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7">
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6">
         <v>1.58</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <v>23.86</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="7">
         <v>0.62</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9" s="7">
         <v>0.214</v>
       </c>
       <c r="P9">
         <v>2</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="Q9" s="8">
         <v>63.81</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9" s="6">
         <v>9.6300000000000008</v>
       </c>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="7">
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="6">
         <v>0.16200000000000001</v>
       </c>
-      <c r="W9" s="10">
+      <c r="W9" s="9">
         <v>66.02</v>
       </c>
-      <c r="X9" s="10">
+      <c r="X9" s="9">
         <v>33.729999999999997</v>
       </c>
-      <c r="Y9" s="10">
+      <c r="Y9" s="9">
         <v>33.200000000000003</v>
       </c>
-      <c r="Z9" s="10">
+      <c r="Z9" s="9">
         <v>25.37</v>
       </c>
-      <c r="AA9" s="10">
+      <c r="AA9" s="9">
         <v>13.38</v>
       </c>
-      <c r="AB9" s="11">
+      <c r="AB9" s="10">
         <v>0.23</v>
       </c>
       <c r="AC9" s="3">
@@ -1417,7 +1584,7 @@
       <c r="AD9" s="3">
         <v>14565</v>
       </c>
-      <c r="AE9" s="12">
+      <c r="AE9" s="11">
         <v>6.95</v>
       </c>
       <c r="AF9" t="s">
@@ -1428,7 +1595,7 @@
       <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>100007</v>
       </c>
       <c r="C10" s="3">
@@ -1440,63 +1607,63 @@
       <c r="E10" s="5">
         <v>0.23599999999999999</v>
       </c>
-      <c r="F10" s="6">
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="F10" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="6">
         <v>0.1149</v>
       </c>
-      <c r="H10" s="6">
-        <v>0.23055555555555554</v>
-      </c>
-      <c r="I10" s="7">
+      <c r="H10" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="I10" s="6">
         <v>0.41</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7">
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6">
         <v>6.39</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <v>40.44</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="7">
         <v>0.36099999999999999</v>
       </c>
-      <c r="O10" s="8">
+      <c r="O10" s="7">
         <v>0.16500000000000001</v>
       </c>
       <c r="P10">
         <v>17</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="Q10" s="8">
         <v>48.2</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="6">
         <v>2.84</v>
       </c>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="7">
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="W10" s="10">
+      <c r="W10" s="9">
         <v>63.85</v>
       </c>
-      <c r="X10" s="10">
+      <c r="X10" s="9">
         <v>38.549999999999997</v>
       </c>
-      <c r="Y10" s="10">
+      <c r="Y10" s="9">
         <v>24.1</v>
       </c>
-      <c r="Z10" s="10">
+      <c r="Z10" s="9">
         <v>26.04</v>
       </c>
-      <c r="AA10" s="10">
+      <c r="AA10" s="9">
         <v>26.85</v>
       </c>
-      <c r="AB10" s="11">
+      <c r="AB10" s="10">
         <v>0.2</v>
       </c>
       <c r="AC10" s="3">
@@ -1505,7 +1672,7 @@
       <c r="AD10" s="3">
         <v>100923</v>
       </c>
-      <c r="AE10" s="12">
+      <c r="AE10" s="11">
         <v>10.01</v>
       </c>
       <c r="AF10" t="s">
@@ -1516,7 +1683,7 @@
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>100008</v>
       </c>
       <c r="C11" s="3">
@@ -1528,68 +1695,68 @@
       <c r="E11" s="5">
         <v>9.3200000000000005E-2</v>
       </c>
-      <c r="F11" s="6">
-        <v>0.22638888888888889</v>
-      </c>
-      <c r="G11" s="7">
+      <c r="F11" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="6">
         <v>0.12659999999999999</v>
       </c>
-      <c r="H11" s="6">
-        <v>0.22569444444444445</v>
-      </c>
-      <c r="I11" s="7">
+      <c r="H11" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11" s="6">
         <v>1.05</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7">
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6">
         <v>1.52</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <v>25.95</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="7">
         <v>0.61</v>
       </c>
-      <c r="O11" s="8">
+      <c r="O11" s="7">
         <v>0.23</v>
       </c>
       <c r="P11">
         <v>5</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="Q11" s="8">
         <v>59.54</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11" s="6">
         <v>4.43</v>
       </c>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="7">
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="6">
         <v>0.72899999999999998</v>
       </c>
-      <c r="W11" s="10">
+      <c r="W11" s="9">
         <v>66.45</v>
       </c>
-      <c r="X11" s="10">
+      <c r="X11" s="9">
         <v>34.56</v>
       </c>
-      <c r="Y11" s="10">
+      <c r="Y11" s="9">
         <v>34.15</v>
       </c>
-      <c r="Z11" s="10">
+      <c r="Z11" s="9">
         <v>24.04</v>
       </c>
-      <c r="AA11" s="10">
+      <c r="AA11" s="9">
         <v>16</v>
       </c>
-      <c r="AB11" s="11">
+      <c r="AB11" s="10">
         <v>0.24</v>
       </c>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
-      <c r="AE11" s="12">
+      <c r="AE11" s="11">
         <v>10.94</v>
       </c>
       <c r="AF11" t="s">
@@ -1600,7 +1767,7 @@
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <v>100009</v>
       </c>
       <c r="C12" s="3">
@@ -1612,72 +1779,72 @@
       <c r="E12" s="5">
         <v>0.1048</v>
       </c>
-      <c r="F12" s="6">
-        <v>0.24097222222222223</v>
-      </c>
-      <c r="G12" s="7">
+      <c r="F12" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="6">
         <v>0.1132</v>
       </c>
-      <c r="H12" s="6">
-        <v>0.19722222222222222</v>
-      </c>
-      <c r="I12" s="7">
+      <c r="H12" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" s="6">
         <v>0.31</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="6">
         <v>0.46</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>0.31</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <v>1.23</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <v>17.43</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="7">
         <v>0.72</v>
       </c>
-      <c r="O12" s="8">
+      <c r="O12" s="7">
         <v>0.24</v>
       </c>
       <c r="P12">
         <v>2</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q12" s="8">
         <v>40</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="6">
         <v>3.28</v>
       </c>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="7">
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="W12" s="10">
+      <c r="W12" s="9">
         <v>74.06</v>
       </c>
-      <c r="X12" s="10">
+      <c r="X12" s="9">
         <v>24.78</v>
       </c>
-      <c r="Y12" s="10">
+      <c r="Y12" s="9">
         <v>39.549999999999997</v>
       </c>
-      <c r="Z12" s="10">
+      <c r="Z12" s="9">
         <v>24.78</v>
       </c>
-      <c r="AA12" s="10">
+      <c r="AA12" s="9">
         <v>16.63</v>
       </c>
-      <c r="AB12" s="11">
+      <c r="AB12" s="10">
         <v>0.23</v>
       </c>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
-      <c r="AE12" s="12">
+      <c r="AE12" s="11">
         <v>6.15</v>
       </c>
       <c r="AF12" t="s">
@@ -1688,7 +1855,7 @@
       <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <v>100010</v>
       </c>
       <c r="C13" s="3">
@@ -1700,63 +1867,63 @@
       <c r="E13" s="5">
         <v>0.21540000000000001</v>
       </c>
-      <c r="F13" s="6">
-        <v>0.17152777777777775</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="F13" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" s="6">
         <v>0.1487</v>
       </c>
-      <c r="H13" s="6">
-        <v>0.26597222222222222</v>
-      </c>
-      <c r="I13" s="7">
+      <c r="H13" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" s="6">
         <v>0.92</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7">
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6">
         <v>5.03</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <v>47.96</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="7">
         <v>0.39</v>
       </c>
-      <c r="O13" s="8">
+      <c r="O13" s="7">
         <v>0.13</v>
       </c>
       <c r="P13">
         <v>1</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="Q13" s="8">
         <v>56</v>
       </c>
-      <c r="R13" s="7">
+      <c r="R13" s="6">
         <v>7.09</v>
       </c>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="7">
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="6">
         <v>0.182</v>
       </c>
-      <c r="W13" s="10">
+      <c r="W13" s="9">
         <v>64.48</v>
       </c>
-      <c r="X13" s="10">
+      <c r="X13" s="9">
         <v>47.18</v>
       </c>
-      <c r="Y13" s="10">
+      <c r="Y13" s="9">
         <v>33.159999999999997</v>
       </c>
-      <c r="Z13" s="10">
+      <c r="Z13" s="9">
         <v>28.71</v>
       </c>
-      <c r="AA13" s="10">
+      <c r="AA13" s="9">
         <v>19.98</v>
       </c>
-      <c r="AB13" s="11">
+      <c r="AB13" s="10">
         <v>0.2</v>
       </c>
       <c r="AC13" s="3">
@@ -1765,7 +1932,7 @@
       <c r="AD13" s="3">
         <v>11275</v>
       </c>
-      <c r="AE13" s="12">
+      <c r="AE13" s="11">
         <v>9.6199999999999992</v>
       </c>
       <c r="AF13" t="s">
@@ -1782,7 +1949,7 @@
   <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H3" sqref="H3:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1892,7 +2059,7 @@
       <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>79</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1984,7 +2151,7 @@
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>100000</v>
       </c>
       <c r="C3" s="3">
@@ -1996,68 +2163,68 @@
       <c r="E3" s="5">
         <v>0.193</v>
       </c>
-      <c r="F3" s="6">
-        <v>0.25972222222222224</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="F3" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="6">
         <v>0.121</v>
       </c>
-      <c r="H3" s="6">
-        <v>0.18263888888888891</v>
-      </c>
-      <c r="I3" s="7">
+      <c r="H3" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="6">
         <v>0.71</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6">
         <v>3.5</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="6">
         <v>38.799999999999997</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="7">
         <v>0.38</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="7">
         <v>0.2</v>
       </c>
       <c r="P3">
         <v>2</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="Q3" s="8">
         <v>44</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3" s="6">
         <v>2.21</v>
       </c>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="7">
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="6">
         <v>0.14099999999999999</v>
       </c>
-      <c r="W3" s="10">
+      <c r="W3" s="9">
         <v>57.16</v>
       </c>
-      <c r="X3" s="10">
+      <c r="X3" s="9">
         <v>44.29</v>
       </c>
-      <c r="Y3" s="10">
+      <c r="Y3" s="9">
         <v>22.18</v>
       </c>
-      <c r="Z3" s="10">
+      <c r="Z3" s="9">
         <v>31.61</v>
       </c>
-      <c r="AA3" s="10">
+      <c r="AA3" s="9">
         <v>20</v>
       </c>
-      <c r="AB3" s="11">
+      <c r="AB3" s="10">
         <v>0.19</v>
       </c>
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
-      <c r="AE3" s="12">
+      <c r="AE3" s="11">
         <v>6.5</v>
       </c>
       <c r="AF3" t="s">
@@ -2068,7 +2235,7 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>100001</v>
       </c>
       <c r="C4" s="3">
@@ -2080,68 +2247,68 @@
       <c r="E4" s="5">
         <v>0.104</v>
       </c>
-      <c r="F4" s="6">
-        <v>0.16527777777777777</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="F4" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="6">
         <v>9.1399999999999995E-2</v>
       </c>
-      <c r="H4" s="6">
-        <v>0.26458333333333334</v>
-      </c>
-      <c r="I4" s="7">
+      <c r="H4" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6">
         <v>1.9</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="6">
         <v>23.3</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="7">
         <v>0.39</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="7">
         <v>0.18</v>
       </c>
       <c r="P4">
         <v>4</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="8">
         <v>59.2</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="6">
         <v>4.9800000000000004</v>
       </c>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="7">
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="6">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="W4" s="10">
+      <c r="W4" s="9">
         <v>43.47</v>
       </c>
-      <c r="X4" s="10">
+      <c r="X4" s="9">
         <v>26.35</v>
       </c>
-      <c r="Y4" s="10">
+      <c r="Y4" s="9">
         <v>24.51</v>
       </c>
-      <c r="Z4" s="10">
+      <c r="Z4" s="9">
         <v>26.35</v>
       </c>
-      <c r="AA4" s="10">
+      <c r="AA4" s="9">
         <v>15.97</v>
       </c>
-      <c r="AB4" s="11">
+      <c r="AB4" s="10">
         <v>0.27</v>
       </c>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
-      <c r="AE4" s="12">
+      <c r="AE4" s="11">
         <v>6.56</v>
       </c>
       <c r="AF4" t="s">
@@ -2152,7 +2319,7 @@
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>100002</v>
       </c>
       <c r="C5" s="3">
@@ -2164,68 +2331,68 @@
       <c r="E5" s="5">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="F5" s="6">
-        <v>0.2076388888888889</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="F5" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="H5" s="6">
-        <v>0.20347222222222219</v>
-      </c>
-      <c r="I5" s="7">
+      <c r="H5" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="I5" s="6">
         <v>0.27</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7">
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6">
         <v>0.9</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="6">
         <v>14.8</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="7">
         <v>0.58599999999999997</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="7">
         <v>0.249</v>
       </c>
       <c r="P5">
         <v>2</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="Q5" s="8">
         <v>58.5</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="6">
         <v>2.57</v>
       </c>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="7">
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="6">
         <v>0.16600000000000001</v>
       </c>
-      <c r="W5" s="10">
+      <c r="W5" s="9">
         <v>40.67</v>
       </c>
-      <c r="X5" s="10">
+      <c r="X5" s="9">
         <v>30.78</v>
       </c>
-      <c r="Y5" s="10">
+      <c r="Y5" s="9">
         <v>24.35</v>
       </c>
-      <c r="Z5" s="10">
+      <c r="Z5" s="9">
         <v>25.82</v>
       </c>
-      <c r="AA5" s="10">
+      <c r="AA5" s="9">
         <v>16</v>
       </c>
-      <c r="AB5" s="11">
+      <c r="AB5" s="10">
         <v>0.21</v>
       </c>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
-      <c r="AE5" s="12">
+      <c r="AE5" s="11">
         <v>5.3</v>
       </c>
       <c r="AF5" t="s">
@@ -2236,7 +2403,7 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>100003</v>
       </c>
       <c r="C6" s="3">
@@ -2248,68 +2415,68 @@
       <c r="E6" s="5">
         <v>0.21</v>
       </c>
-      <c r="F6" s="6">
-        <v>0.19722222222222222</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="F6" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="6">
         <v>0.12039999999999999</v>
       </c>
-      <c r="H6" s="6">
-        <v>0.21458333333333335</v>
-      </c>
-      <c r="I6" s="7">
+      <c r="H6" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="6">
         <v>0.76</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7">
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6">
         <v>4.18</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="6">
         <v>57.5</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="7">
         <v>0.377</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <v>0.1</v>
       </c>
       <c r="P6">
         <v>3</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="Q6" s="8">
         <v>35.6</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="6">
         <v>8.43</v>
       </c>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="7">
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="6">
         <v>0.19800000000000001</v>
       </c>
-      <c r="W6" s="10">
+      <c r="W6" s="9">
         <v>61.88</v>
       </c>
-      <c r="X6" s="10">
+      <c r="X6" s="9">
         <v>51.92</v>
       </c>
-      <c r="Y6" s="10">
+      <c r="Y6" s="9">
         <v>33.18</v>
       </c>
-      <c r="Z6" s="10">
+      <c r="Z6" s="9">
         <v>37.68</v>
       </c>
-      <c r="AA6" s="10">
+      <c r="AA6" s="9">
         <v>16.3</v>
       </c>
-      <c r="AB6" s="11">
+      <c r="AB6" s="10">
         <v>0.16</v>
       </c>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="12">
+      <c r="AE6" s="11">
         <v>7.42</v>
       </c>
       <c r="AF6" t="s">
@@ -2320,7 +2487,7 @@
       <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>100004</v>
       </c>
       <c r="C7" s="3">
@@ -2332,68 +2499,68 @@
       <c r="E7" s="5">
         <v>0.121</v>
       </c>
-      <c r="F7" s="6">
-        <v>0.21041666666666667</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="F7" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="6">
         <v>6.5600000000000006E-2</v>
       </c>
-      <c r="H7" s="6">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="I7" s="7">
+      <c r="H7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="6">
         <v>0.3</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7">
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6">
         <v>1.49</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <v>21.2</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="7">
         <v>0.44</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="7">
         <v>0.17</v>
       </c>
       <c r="P7">
         <v>1</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="8">
         <v>48</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="6">
         <v>4.51</v>
       </c>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="7">
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="6">
         <v>9.4E-2</v>
       </c>
-      <c r="W7" s="10">
+      <c r="W7" s="9">
         <v>70.34</v>
       </c>
-      <c r="X7" s="10">
+      <c r="X7" s="9">
         <v>104.78</v>
       </c>
-      <c r="Y7" s="10">
+      <c r="Y7" s="9">
         <v>32.5</v>
       </c>
-      <c r="Z7" s="10">
+      <c r="Z7" s="9">
         <v>69.349999999999994</v>
       </c>
-      <c r="AA7" s="10">
+      <c r="AA7" s="9">
         <v>22.8</v>
       </c>
-      <c r="AB7" s="11">
+      <c r="AB7" s="10">
         <v>0.248</v>
       </c>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
-      <c r="AE7" s="12">
+      <c r="AE7" s="11">
         <v>6.91</v>
       </c>
       <c r="AF7" t="s">
@@ -2404,7 +2571,7 @@
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>100005</v>
       </c>
       <c r="C8" s="3">
@@ -2416,68 +2583,68 @@
       <c r="E8" s="5">
         <v>0.151</v>
       </c>
-      <c r="F8" s="6">
-        <v>0.21180555555555555</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="F8" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="6">
         <v>0.1263</v>
       </c>
-      <c r="H8" s="6">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="I8" s="7">
+      <c r="H8" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="I8" s="6">
         <v>0.64</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7">
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6">
         <v>4.6500000000000004</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <v>28.6</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="7">
         <v>0.48099999999999998</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="7">
         <v>0.33</v>
       </c>
       <c r="P8">
         <v>4</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="Q8" s="8">
         <v>54</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="6">
         <v>4</v>
       </c>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="7">
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="6">
         <v>0.13</v>
       </c>
-      <c r="W8" s="10">
+      <c r="W8" s="9">
         <v>77.650000000000006</v>
       </c>
-      <c r="X8" s="10">
+      <c r="X8" s="9">
         <v>49.17</v>
       </c>
-      <c r="Y8" s="10">
+      <c r="Y8" s="9">
         <v>46.63</v>
       </c>
-      <c r="Z8" s="10">
+      <c r="Z8" s="9">
         <v>43.53</v>
       </c>
-      <c r="AA8" s="10">
+      <c r="AA8" s="9">
         <v>26.1</v>
       </c>
-      <c r="AB8" s="11">
+      <c r="AB8" s="10">
         <v>0.26</v>
       </c>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
-      <c r="AE8" s="12">
+      <c r="AE8" s="11">
         <v>8.32</v>
       </c>
       <c r="AF8" t="s">
@@ -2488,7 +2655,7 @@
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>100006</v>
       </c>
       <c r="C9" s="3">
@@ -2500,63 +2667,63 @@
       <c r="E9" s="5">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="F9" s="6">
-        <v>0.23194444444444443</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="F9" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" s="6">
         <v>0.10199999999999999</v>
       </c>
-      <c r="H9" s="6">
-        <v>0.27847222222222223</v>
-      </c>
-      <c r="I9" s="7">
+      <c r="H9" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" s="6">
         <v>0.31</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7">
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6">
         <v>1.46</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <v>19.7</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="7">
         <v>0.6</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9" s="7">
         <v>0.21</v>
       </c>
       <c r="P9">
         <v>2</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="Q9" s="8">
         <v>63.8</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9" s="6">
         <v>9.24</v>
       </c>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="7">
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="6">
         <v>0.16500000000000001</v>
       </c>
-      <c r="W9" s="10">
+      <c r="W9" s="9">
         <v>66.02</v>
       </c>
-      <c r="X9" s="10">
+      <c r="X9" s="9">
         <v>33.729999999999997</v>
       </c>
-      <c r="Y9" s="10">
+      <c r="Y9" s="9">
         <v>32.5</v>
       </c>
-      <c r="Z9" s="10">
+      <c r="Z9" s="9">
         <v>25.37</v>
       </c>
-      <c r="AA9" s="10">
+      <c r="AA9" s="9">
         <v>13.38</v>
       </c>
-      <c r="AB9" s="11">
+      <c r="AB9" s="10">
         <v>0.23</v>
       </c>
       <c r="AC9" s="3">
@@ -2565,7 +2732,7 @@
       <c r="AD9" s="3">
         <v>15581</v>
       </c>
-      <c r="AE9" s="12">
+      <c r="AE9" s="11">
         <v>6.55</v>
       </c>
       <c r="AF9" t="s">
@@ -2576,7 +2743,7 @@
       <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>100007</v>
       </c>
       <c r="C10" s="3">
@@ -2588,63 +2755,63 @@
       <c r="E10" s="5">
         <v>0.23300000000000001</v>
       </c>
-      <c r="F10" s="6">
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="F10" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="6">
         <v>0.1149</v>
       </c>
-      <c r="H10" s="6">
-        <v>0.24305555555555555</v>
-      </c>
-      <c r="I10" s="7">
+      <c r="H10" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" s="6">
         <v>0.43</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7">
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6">
         <v>5.9</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <v>38.799999999999997</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="7">
         <v>0.32900000000000001</v>
       </c>
-      <c r="O10" s="8">
+      <c r="O10" s="7">
         <v>0.17</v>
       </c>
       <c r="P10">
         <v>17</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="Q10" s="8">
         <v>48.24</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="6">
         <v>2.84</v>
       </c>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="7">
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="W10" s="10">
+      <c r="W10" s="9">
         <v>63.85</v>
       </c>
-      <c r="X10" s="10">
+      <c r="X10" s="9">
         <v>38.549999999999997</v>
       </c>
-      <c r="Y10" s="10">
+      <c r="Y10" s="9">
         <v>24.1</v>
       </c>
-      <c r="Z10" s="10">
+      <c r="Z10" s="9">
         <v>26.04</v>
       </c>
-      <c r="AA10" s="10">
+      <c r="AA10" s="9">
         <v>26.85</v>
       </c>
-      <c r="AB10" s="11">
+      <c r="AB10" s="10">
         <v>0.2</v>
       </c>
       <c r="AC10" s="3">
@@ -2653,7 +2820,7 @@
       <c r="AD10" s="3">
         <v>118476</v>
       </c>
-      <c r="AE10" s="12">
+      <c r="AE10" s="11">
         <v>9.82</v>
       </c>
       <c r="AF10" t="s">
@@ -2664,7 +2831,7 @@
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>100008</v>
       </c>
       <c r="C11" s="3">
@@ -2676,68 +2843,68 @@
       <c r="E11" s="5">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="F11" s="6">
-        <v>0.22569444444444445</v>
-      </c>
-      <c r="G11" s="7">
+      <c r="F11" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="6">
         <v>0.1434</v>
       </c>
-      <c r="H11" s="6">
-        <v>0.21666666666666667</v>
-      </c>
-      <c r="I11" s="7">
+      <c r="H11" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="I11" s="6">
         <v>1.05</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7">
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6">
         <v>1.63</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <v>23.9</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="7">
         <v>0.57999999999999996</v>
       </c>
-      <c r="O11" s="8">
+      <c r="O11" s="7">
         <v>0.27</v>
       </c>
       <c r="P11">
         <v>5</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="Q11" s="8">
         <v>59.5</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11" s="6">
         <v>4.43</v>
       </c>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="7">
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="6">
         <v>0.73099999999999998</v>
       </c>
-      <c r="W11" s="10">
+      <c r="W11" s="9">
         <v>66.45</v>
       </c>
-      <c r="X11" s="10">
+      <c r="X11" s="9">
         <v>34.56</v>
       </c>
-      <c r="Y11" s="10">
+      <c r="Y11" s="9">
         <v>34.15</v>
       </c>
-      <c r="Z11" s="10">
+      <c r="Z11" s="9">
         <v>24.04</v>
       </c>
-      <c r="AA11" s="10">
+      <c r="AA11" s="9">
         <v>16</v>
       </c>
-      <c r="AB11" s="11">
+      <c r="AB11" s="10">
         <v>0.28000000000000003</v>
       </c>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
-      <c r="AE11" s="12">
+      <c r="AE11" s="11">
         <v>10.72</v>
       </c>
       <c r="AF11" t="s">
@@ -2748,7 +2915,7 @@
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <v>100009</v>
       </c>
       <c r="C12" s="3">
@@ -2760,67 +2927,67 @@
       <c r="E12" s="5">
         <v>0.122</v>
       </c>
-      <c r="F12" s="6">
-        <v>0.22777777777777777</v>
-      </c>
-      <c r="G12" s="7">
+      <c r="F12" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="6">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="H12" s="6">
-        <v>0.19166666666666665</v>
-      </c>
-      <c r="I12" s="7">
+      <c r="H12" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="I12" s="6">
         <v>0.31</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="6">
         <v>0.47</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>0.31</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <v>1.6</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <v>22.3</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="7">
         <v>0.57899999999999996</v>
       </c>
-      <c r="O12" s="8">
+      <c r="O12" s="7">
         <v>0.21299999999999999</v>
       </c>
       <c r="P12">
         <v>2</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q12" s="8">
         <v>40</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="6">
         <v>3.28</v>
       </c>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="7">
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="W12" s="10">
+      <c r="W12" s="9">
         <v>74.06</v>
       </c>
-      <c r="X12" s="10">
+      <c r="X12" s="9">
         <v>24.78</v>
       </c>
-      <c r="Y12" s="10">
+      <c r="Y12" s="9">
         <v>39.549999999999997</v>
       </c>
-      <c r="Z12" s="10">
+      <c r="Z12" s="9">
         <v>24.78</v>
       </c>
-      <c r="AA12" s="10">
+      <c r="AA12" s="9">
         <v>16.63</v>
       </c>
-      <c r="AB12" s="11">
+      <c r="AB12" s="10">
         <v>0.22</v>
       </c>
       <c r="AC12" s="3">
@@ -2829,7 +2996,7 @@
       <c r="AD12" s="3">
         <v>9562</v>
       </c>
-      <c r="AE12" s="12">
+      <c r="AE12" s="11">
         <v>6.3</v>
       </c>
       <c r="AF12" t="s">
@@ -2840,7 +3007,7 @@
       <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <v>100010</v>
       </c>
       <c r="C13" s="3">
@@ -2852,63 +3019,63 @@
       <c r="E13" s="5">
         <v>0.23300000000000001</v>
       </c>
-      <c r="F13" s="6">
-        <v>0.17569444444444446</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="F13" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" s="6">
         <v>0.13789999999999999</v>
       </c>
-      <c r="H13" s="6">
-        <v>0.27499999999999997</v>
-      </c>
-      <c r="I13" s="7">
+      <c r="H13" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" s="6">
         <v>0.88</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7">
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6">
         <v>4.71</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <v>47.7</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="7">
         <v>0.31900000000000001</v>
       </c>
-      <c r="O13" s="8">
+      <c r="O13" s="7">
         <v>0.11799999999999999</v>
       </c>
       <c r="P13">
         <v>1</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="Q13" s="8">
         <v>56</v>
       </c>
-      <c r="R13" s="7">
+      <c r="R13" s="6">
         <v>7.09</v>
       </c>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="7">
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="6">
         <v>0.17699999999999999</v>
       </c>
-      <c r="W13" s="10">
+      <c r="W13" s="9">
         <v>64.48</v>
       </c>
-      <c r="X13" s="10">
+      <c r="X13" s="9">
         <v>47.18</v>
       </c>
-      <c r="Y13" s="10">
+      <c r="Y13" s="9">
         <v>33.159999999999997</v>
       </c>
-      <c r="Z13" s="10">
+      <c r="Z13" s="9">
         <v>28.71</v>
       </c>
-      <c r="AA13" s="10">
+      <c r="AA13" s="9">
         <v>19.98</v>
       </c>
-      <c r="AB13" s="11">
+      <c r="AB13" s="10">
         <v>0.19</v>
       </c>
       <c r="AC13" s="3">
@@ -2917,7 +3084,7 @@
       <c r="AD13" s="3">
         <v>11135</v>
       </c>
-      <c r="AE13" s="12">
+      <c r="AE13" s="11">
         <v>9.36</v>
       </c>
       <c r="AF13" t="s">
@@ -2933,11 +3100,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="20.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -3044,7 +3214,7 @@
       <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>79</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -3136,7 +3306,7 @@
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>100000</v>
       </c>
       <c r="C3" s="3">
@@ -3148,73 +3318,73 @@
       <c r="E3" s="5">
         <v>0.16200000000000001</v>
       </c>
-      <c r="F3" s="6">
-        <v>0.25833333333333336</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="F3" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="6">
         <v>0.13305358860040215</v>
       </c>
-      <c r="H3" s="6">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="I3" s="7">
+      <c r="H3" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="6">
         <v>0.93</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="6">
         <v>0.25</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>0.68</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="6">
         <v>3.4843205574912894</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="6">
         <v>38.664718444419471</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="7">
         <v>0.38</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="7">
         <v>0.17</v>
       </c>
       <c r="P3">
         <v>2</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="Q3" s="8">
         <v>43</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3" s="6">
         <v>2.96</v>
       </c>
-      <c r="S3" s="9">
+      <c r="S3" s="8">
         <v>112</v>
       </c>
-      <c r="T3" s="9">
+      <c r="T3" s="8">
         <v>45</v>
       </c>
-      <c r="U3" s="9">
+      <c r="U3" s="8">
         <v>80</v>
       </c>
-      <c r="V3" s="7">
+      <c r="V3" s="6">
         <v>0.187</v>
       </c>
-      <c r="W3" s="10">
+      <c r="W3" s="9">
         <v>57.16</v>
       </c>
-      <c r="X3" s="10">
+      <c r="X3" s="9">
         <v>44.29</v>
       </c>
-      <c r="Y3" s="10">
+      <c r="Y3" s="9">
         <v>22.18</v>
       </c>
-      <c r="Z3" s="10">
+      <c r="Z3" s="9">
         <v>31.61</v>
       </c>
-      <c r="AA3" s="10">
+      <c r="AA3" s="9">
         <v>20</v>
       </c>
-      <c r="AB3" s="11">
+      <c r="AB3" s="10">
         <v>0.159</v>
       </c>
       <c r="AC3" s="3">
@@ -3223,7 +3393,7 @@
       <c r="AD3" s="3">
         <v>5970</v>
       </c>
-      <c r="AE3" s="12">
+      <c r="AE3" s="11">
         <v>6.334844454435328</v>
       </c>
       <c r="AF3" t="s">
@@ -3234,7 +3404,7 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>100001</v>
       </c>
       <c r="C4" s="3">
@@ -3246,73 +3416,73 @@
       <c r="E4" s="5">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="F4" s="6">
-        <v>0.15833333333333333</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="F4" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="6">
         <v>9.577444551321708E-2</v>
       </c>
-      <c r="H4" s="6">
-        <v>0.25625000000000003</v>
-      </c>
-      <c r="I4" s="7">
+      <c r="H4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" s="6">
         <v>0.58066949514462363</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <v>0.16441226596207498</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>0.41625722918254859</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="6">
         <v>1.9557208827086334</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="6">
         <v>21.524903511117675</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="7">
         <v>0.46</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="7">
         <v>0.22</v>
       </c>
       <c r="P4">
         <v>4</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="8">
         <v>61.18</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="6">
         <v>6.16</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4" s="8">
         <v>1242.19</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T4" s="8">
         <v>301.7</v>
       </c>
-      <c r="U4" s="9">
+      <c r="U4" s="8">
         <v>0</v>
       </c>
-      <c r="V4" s="7">
+      <c r="V4" s="6">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="W4" s="10">
+      <c r="W4" s="9">
         <v>43.47</v>
       </c>
-      <c r="X4" s="10">
+      <c r="X4" s="9">
         <v>26.35</v>
       </c>
-      <c r="Y4" s="10">
+      <c r="Y4" s="9">
         <v>24.51</v>
       </c>
-      <c r="Z4" s="10">
+      <c r="Z4" s="9">
         <v>26.35</v>
       </c>
-      <c r="AA4" s="10">
+      <c r="AA4" s="9">
         <v>15.97</v>
       </c>
-      <c r="AB4" s="11">
+      <c r="AB4" s="10">
         <v>0.27</v>
       </c>
       <c r="AC4" s="3">
@@ -3321,7 +3491,7 @@
       <c r="AD4" s="3">
         <v>22229</v>
       </c>
-      <c r="AE4" s="12">
+      <c r="AE4" s="11">
         <v>6.5264002362830134</v>
       </c>
       <c r="AF4" t="s">
@@ -3332,7 +3502,7 @@
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>100002</v>
       </c>
       <c r="C5" s="3">
@@ -3344,73 +3514,73 @@
       <c r="E5" s="5">
         <v>0.06</v>
       </c>
-      <c r="F5" s="6">
-        <v>0.22083333333333333</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="F5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="6">
         <v>7.8868508029391785E-2</v>
       </c>
-      <c r="H5" s="6">
-        <v>0.17430555555555557</v>
-      </c>
-      <c r="I5" s="7">
+      <c r="H5" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" s="6">
         <v>0.28594054123893953</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="6">
         <v>0.47</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
         <v>0.73771209222651513</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="6">
         <v>13.616414719231779</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="7">
         <v>0.58699999999999997</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="7">
         <v>0.251</v>
       </c>
       <c r="P5">
         <v>2</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="Q5" s="8">
         <v>55</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="6">
         <v>3.93</v>
       </c>
-      <c r="S5" s="9">
+      <c r="S5" s="8">
         <v>605</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="8">
         <v>337</v>
       </c>
-      <c r="U5" s="9">
+      <c r="U5" s="8">
         <v>0</v>
       </c>
-      <c r="V5" s="7">
+      <c r="V5" s="6">
         <v>0.16300000000000001</v>
       </c>
-      <c r="W5" s="10">
+      <c r="W5" s="9">
         <v>40.67</v>
       </c>
-      <c r="X5" s="10">
+      <c r="X5" s="9">
         <v>30.78</v>
       </c>
-      <c r="Y5" s="10">
+      <c r="Y5" s="9">
         <v>24.35</v>
       </c>
-      <c r="Z5" s="10">
+      <c r="Z5" s="9">
         <v>25.82</v>
       </c>
-      <c r="AA5" s="10">
+      <c r="AA5" s="9">
         <v>16</v>
       </c>
-      <c r="AB5" s="11">
+      <c r="AB5" s="10">
         <v>0.21340000000000001</v>
       </c>
       <c r="AC5" s="3">
@@ -3419,7 +3589,7 @@
       <c r="AD5" s="3">
         <v>19924</v>
       </c>
-      <c r="AE5" s="12">
+      <c r="AE5" s="11">
         <v>5.44</v>
       </c>
       <c r="AF5" t="s">
@@ -3430,7 +3600,7 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>100003</v>
       </c>
       <c r="C6" s="3">
@@ -3442,73 +3612,73 @@
       <c r="E6" s="5">
         <v>0.22500000000000001</v>
       </c>
-      <c r="F6" s="6">
-        <v>0.20902777777777778</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="F6" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="6">
         <v>9.4336685974853091E-2</v>
       </c>
-      <c r="H6" s="6">
-        <v>0.25486111111111115</v>
-      </c>
-      <c r="I6" s="7">
+      <c r="H6" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" s="6">
         <v>0.49375954367057456</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>0.32</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <v>3.9668016977742999</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="6">
         <v>54.49619935807641</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="7">
         <v>0.3</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <v>0.19</v>
       </c>
       <c r="P6">
         <v>3</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="Q6" s="8">
         <v>36.9</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="6">
         <v>9.17</v>
       </c>
-      <c r="S6" s="9">
+      <c r="S6" s="8">
         <v>965</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6" s="8">
         <v>115</v>
       </c>
-      <c r="U6" s="9">
+      <c r="U6" s="8">
         <v>1100</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="6">
         <v>0.19800000000000001</v>
       </c>
-      <c r="W6" s="10">
+      <c r="W6" s="9">
         <v>61.88</v>
       </c>
-      <c r="X6" s="10">
+      <c r="X6" s="9">
         <v>51.92</v>
       </c>
-      <c r="Y6" s="10">
+      <c r="Y6" s="9">
         <v>33.18</v>
       </c>
-      <c r="Z6" s="10">
+      <c r="Z6" s="9">
         <v>37.68</v>
       </c>
-      <c r="AA6" s="10">
+      <c r="AA6" s="9">
         <v>16.3</v>
       </c>
-      <c r="AB6" s="11">
+      <c r="AB6" s="10">
         <v>0.16</v>
       </c>
       <c r="AC6" s="3">
@@ -3517,7 +3687,7 @@
       <c r="AD6" s="3">
         <v>14775</v>
       </c>
-      <c r="AE6" s="12">
+      <c r="AE6" s="11">
         <v>7.3289080147903229</v>
       </c>
       <c r="AF6" t="s">
@@ -3528,7 +3698,7 @@
       <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>100004</v>
       </c>
       <c r="C7" s="3">
@@ -3540,73 +3710,73 @@
       <c r="E7" s="5">
         <v>0.09</v>
       </c>
-      <c r="F7" s="6">
-        <v>0.26874999999999999</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="F7" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="6">
         <v>8.765938942818044E-2</v>
       </c>
-      <c r="H7" s="6">
-        <v>0.13541666666666666</v>
-      </c>
-      <c r="I7" s="7">
+      <c r="H7" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="6">
         <v>0.58868894601542421</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <v>0.27708501195820384</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>0.31160393405722031</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <v>1.8289017636751974</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <v>22.816508716059804</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="7">
         <v>0.16</v>
       </c>
       <c r="P7">
         <v>1</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="8">
         <v>48</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="6">
         <v>7.43</v>
       </c>
-      <c r="S7" s="9">
+      <c r="S7" s="8">
         <v>212</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="8">
         <v>224</v>
       </c>
-      <c r="U7" s="9">
+      <c r="U7" s="8">
         <v>145</v>
       </c>
-      <c r="V7" s="7">
+      <c r="V7" s="6">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="W7" s="10">
+      <c r="W7" s="9">
         <v>70.34</v>
       </c>
-      <c r="X7" s="10">
+      <c r="X7" s="9">
         <v>104.78</v>
       </c>
-      <c r="Y7" s="10">
+      <c r="Y7" s="9">
         <v>32.5</v>
       </c>
-      <c r="Z7" s="10">
+      <c r="Z7" s="9">
         <v>69.349999999999994</v>
       </c>
-      <c r="AA7" s="10">
+      <c r="AA7" s="9">
         <v>22.8</v>
       </c>
-      <c r="AB7" s="11">
+      <c r="AB7" s="10">
         <v>0.24179999999999999</v>
       </c>
       <c r="AC7" s="3">
@@ -3615,7 +3785,7 @@
       <c r="AD7" s="3">
         <v>7549.09</v>
       </c>
-      <c r="AE7" s="12">
+      <c r="AE7" s="11">
         <v>6.7912366189617472</v>
       </c>
       <c r="AF7" t="s">
@@ -3626,7 +3796,7 @@
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>100005</v>
       </c>
       <c r="C8" s="3">
@@ -3638,73 +3808,73 @@
       <c r="E8" s="5">
         <v>0.17199999999999999</v>
       </c>
-      <c r="F8" s="6">
-        <v>0.22083333333333333</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="F8" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="6">
         <v>0.14013586235808459</v>
       </c>
-      <c r="H8" s="6">
-        <v>0.16250000000000001</v>
-      </c>
-      <c r="I8" s="7">
+      <c r="H8" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="6">
         <v>0.65</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <v>0.36</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="6">
         <v>4.2178931067819958</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <v>25.463497685719908</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="7">
         <v>0.50070000000000003</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="7">
         <v>0.29189999999999999</v>
       </c>
       <c r="P8">
         <v>4</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="Q8" s="8">
         <v>60</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="6">
         <v>5.13</v>
       </c>
-      <c r="S8" s="9">
+      <c r="S8" s="8">
         <v>1924</v>
       </c>
-      <c r="T8" s="9">
+      <c r="T8" s="8">
         <v>475</v>
       </c>
-      <c r="U8" s="9">
+      <c r="U8" s="8">
         <v>0</v>
       </c>
-      <c r="V8" s="7">
+      <c r="V8" s="6">
         <v>0.128</v>
       </c>
-      <c r="W8" s="10">
+      <c r="W8" s="9">
         <v>80.81</v>
       </c>
-      <c r="X8" s="10">
+      <c r="X8" s="9">
         <v>49.17</v>
       </c>
-      <c r="Y8" s="10">
+      <c r="Y8" s="9">
         <v>44.46</v>
       </c>
-      <c r="Z8" s="10">
+      <c r="Z8" s="9">
         <v>43.53</v>
       </c>
-      <c r="AA8" s="10">
+      <c r="AA8" s="9">
         <v>28.63</v>
       </c>
-      <c r="AB8" s="11">
+      <c r="AB8" s="10">
         <v>0.24</v>
       </c>
       <c r="AC8" s="3">
@@ -3713,7 +3883,7 @@
       <c r="AD8" s="3">
         <v>56101</v>
       </c>
-      <c r="AE8" s="12">
+      <c r="AE8" s="11">
         <v>7.93</v>
       </c>
       <c r="AF8" t="s">
@@ -3724,7 +3894,7 @@
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>100006</v>
       </c>
       <c r="C9" s="3">
@@ -3736,69 +3906,69 @@
       <c r="E9" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F9" s="6">
-        <v>0.24027777777777778</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="F9" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="6">
         <v>0.14134898065927987</v>
       </c>
-      <c r="H9" s="6">
-        <v>0.29236111111111113</v>
-      </c>
-      <c r="I9" s="7">
+      <c r="H9" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="6">
         <v>0.32017699434267405</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7">
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6">
         <v>1.7014062152429164</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <v>20.248537572219583</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="7">
         <v>0.56999999999999995</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9" s="7">
         <v>0.21</v>
       </c>
       <c r="P9">
         <v>2</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="Q9" s="8">
         <v>66</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9" s="6">
         <v>8.8000000000000007</v>
       </c>
-      <c r="S9" s="9">
+      <c r="S9" s="8">
         <v>445</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="8">
         <v>120</v>
       </c>
-      <c r="U9" s="9">
+      <c r="U9" s="8">
         <v>898</v>
       </c>
-      <c r="V9" s="7">
+      <c r="V9" s="6">
         <v>0.16200000000000001</v>
       </c>
-      <c r="W9" s="10">
+      <c r="W9" s="9">
         <v>66.02</v>
       </c>
-      <c r="X9" s="10">
+      <c r="X9" s="9">
         <v>33.729999999999997</v>
       </c>
-      <c r="Y9" s="10">
+      <c r="Y9" s="9">
         <v>33.200000000000003</v>
       </c>
-      <c r="Z9" s="10">
+      <c r="Z9" s="9">
         <v>25.37</v>
       </c>
-      <c r="AA9" s="10">
+      <c r="AA9" s="9">
         <v>13.1</v>
       </c>
-      <c r="AB9" s="11">
+      <c r="AB9" s="10">
         <v>0.23</v>
       </c>
       <c r="AC9" s="3">
@@ -3807,7 +3977,7 @@
       <c r="AD9" s="3">
         <v>15857</v>
       </c>
-      <c r="AE9" s="12">
+      <c r="AE9" s="11">
         <v>6.88750879260279</v>
       </c>
       <c r="AF9" t="s">
@@ -3818,7 +3988,7 @@
       <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>100007</v>
       </c>
       <c r="C10" s="3">
@@ -3830,73 +4000,73 @@
       <c r="E10" s="5">
         <v>0.223</v>
       </c>
-      <c r="F10" s="6">
-        <v>0.18680555555555556</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="F10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" s="6">
         <v>0.1255</v>
       </c>
-      <c r="H10" s="6">
-        <v>0.25833333333333336</v>
-      </c>
-      <c r="I10" s="7">
+      <c r="H10" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" s="6">
         <v>0.53</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="6">
         <v>0.1</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <v>0.43</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="6">
         <v>5.936462353046756</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <v>34.907244778913089</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="O10" s="8">
+      <c r="O10" s="7">
         <v>0.16</v>
       </c>
       <c r="P10">
         <v>17</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="Q10" s="8">
         <v>48.24</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="6">
         <v>30.57</v>
       </c>
-      <c r="S10" s="9">
+      <c r="S10" s="8">
         <v>5148</v>
       </c>
-      <c r="T10" s="9">
+      <c r="T10" s="8">
         <v>1106</v>
       </c>
-      <c r="U10" s="9">
+      <c r="U10" s="8">
         <v>41440</v>
       </c>
-      <c r="V10" s="7">
+      <c r="V10" s="6">
         <v>0.28799999999999998</v>
       </c>
-      <c r="W10" s="10">
+      <c r="W10" s="9">
         <v>66.150000000000006</v>
       </c>
-      <c r="X10" s="10">
+      <c r="X10" s="9">
         <v>41.41</v>
       </c>
-      <c r="Y10" s="10">
+      <c r="Y10" s="9">
         <v>24.74</v>
       </c>
-      <c r="Z10" s="10">
+      <c r="Z10" s="9">
         <v>27.94</v>
       </c>
-      <c r="AA10" s="10">
+      <c r="AA10" s="9">
         <v>26.85</v>
       </c>
-      <c r="AB10" s="11">
+      <c r="AB10" s="10">
         <v>0.2</v>
       </c>
       <c r="AC10" s="3">
@@ -3905,7 +4075,7 @@
       <c r="AD10" s="3">
         <v>136486</v>
       </c>
-      <c r="AE10" s="12">
+      <c r="AE10" s="11">
         <v>9.4</v>
       </c>
       <c r="AF10" t="s">
@@ -3916,7 +4086,7 @@
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>100008</v>
       </c>
       <c r="C11" s="3">
@@ -3928,73 +4098,73 @@
       <c r="E11" s="5">
         <v>0.11</v>
       </c>
-      <c r="F11" s="6">
-        <v>0.18888888888888888</v>
-      </c>
-      <c r="G11" s="7">
+      <c r="F11" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="6">
         <v>0.1474897990914783</v>
       </c>
-      <c r="H11" s="6">
-        <v>0.21597222222222223</v>
-      </c>
-      <c r="I11" s="7">
+      <c r="H11" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="6">
         <v>0.5178909858006715</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>0.55666494375317799</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="6">
         <v>1.8237669612428511</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <v>22.406279809555027</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="7">
         <v>0.52</v>
       </c>
-      <c r="O11" s="8">
+      <c r="O11" s="7">
         <v>0.3</v>
       </c>
       <c r="P11">
         <v>5</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="Q11" s="8">
         <v>61.95</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11" s="6">
         <v>132.51</v>
       </c>
-      <c r="S11" s="9">
+      <c r="S11" s="8">
         <v>974.4</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="8">
         <v>0</v>
       </c>
-      <c r="U11" s="9">
+      <c r="U11" s="8">
         <v>30560</v>
       </c>
-      <c r="V11" s="7">
+      <c r="V11" s="6">
         <v>0.504</v>
       </c>
-      <c r="W11" s="10">
+      <c r="W11" s="9">
         <v>66.45</v>
       </c>
-      <c r="X11" s="10">
+      <c r="X11" s="9">
         <v>34.56</v>
       </c>
-      <c r="Y11" s="10">
+      <c r="Y11" s="9">
         <v>34.15</v>
       </c>
-      <c r="Z11" s="10">
+      <c r="Z11" s="9">
         <v>24.04</v>
       </c>
-      <c r="AA11" s="10">
+      <c r="AA11" s="9">
         <v>16</v>
       </c>
-      <c r="AB11" s="11">
+      <c r="AB11" s="10">
         <v>0.28000000000000003</v>
       </c>
       <c r="AC11" s="3">
@@ -4003,7 +4173,7 @@
       <c r="AD11" s="3">
         <v>24212</v>
       </c>
-      <c r="AE11" s="12">
+      <c r="AE11" s="11">
         <v>10.40156490971513</v>
       </c>
       <c r="AF11" t="s">
@@ -4014,7 +4184,7 @@
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <v>100009</v>
       </c>
       <c r="C12" s="3">
@@ -4026,73 +4196,73 @@
       <c r="E12" s="5">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="F12" s="6">
-        <v>0.24305555555555555</v>
-      </c>
-      <c r="G12" s="7">
+      <c r="F12" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" s="6">
         <v>0.13181257898924967</v>
       </c>
-      <c r="H12" s="6">
-        <v>0.21041666666666667</v>
-      </c>
-      <c r="I12" s="7">
+      <c r="H12" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="6">
         <v>0.30824140674977768</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="6">
         <v>0.37</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>0.31</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <v>1.3106364388135621</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <v>17.022670889828525</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="7">
         <v>0.65</v>
       </c>
-      <c r="O12" s="8">
+      <c r="O12" s="7">
         <v>0.24</v>
       </c>
       <c r="P12">
         <v>2</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q12" s="8">
         <v>68</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="6">
         <v>2.62</v>
       </c>
-      <c r="S12" s="9">
+      <c r="S12" s="8">
         <v>0</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="8">
         <v>336</v>
       </c>
-      <c r="U12" s="9">
+      <c r="U12" s="8">
         <v>0</v>
       </c>
-      <c r="V12" s="7">
+      <c r="V12" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="W12" s="10">
+      <c r="W12" s="9">
         <v>74.06</v>
       </c>
-      <c r="X12" s="10">
+      <c r="X12" s="9">
         <v>24.78</v>
       </c>
-      <c r="Y12" s="10">
+      <c r="Y12" s="9">
         <v>39.549999999999997</v>
       </c>
-      <c r="Z12" s="10">
+      <c r="Z12" s="9">
         <v>24.78</v>
       </c>
-      <c r="AA12" s="10">
+      <c r="AA12" s="9">
         <v>16.16</v>
       </c>
-      <c r="AB12" s="11">
+      <c r="AB12" s="10">
         <v>0.22</v>
       </c>
       <c r="AC12" s="3">
@@ -4101,7 +4271,7 @@
       <c r="AD12" s="3">
         <v>9597</v>
       </c>
-      <c r="AE12" s="12">
+      <c r="AE12" s="11">
         <v>6.2692109656582051</v>
       </c>
       <c r="AF12" t="s">
@@ -4112,7 +4282,7 @@
       <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <v>100010</v>
       </c>
       <c r="C13" s="3">
@@ -4124,73 +4294,73 @@
       <c r="E13" s="5">
         <v>0.2</v>
       </c>
-      <c r="F13" s="6">
-        <v>0.17777777777777778</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="F13" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="6">
         <v>0.13500000000000001</v>
       </c>
-      <c r="H13" s="6">
-        <v>0.27152777777777776</v>
-      </c>
-      <c r="I13" s="7">
+      <c r="H13" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="6">
         <v>0.76</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="6">
         <v>0.19</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="6">
         <v>4.0830426312689712</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <v>43.276854075114393</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="7">
         <v>0.38279999999999997</v>
       </c>
-      <c r="O13" s="8">
+      <c r="O13" s="7">
         <v>0.1182</v>
       </c>
       <c r="P13">
         <v>1</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="Q13" s="8">
         <v>61</v>
       </c>
-      <c r="R13" s="7">
+      <c r="R13" s="6">
         <v>9.1300000000000008</v>
       </c>
-      <c r="S13" s="9">
+      <c r="S13" s="8">
         <v>1290</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13" s="8">
         <v>0</v>
       </c>
-      <c r="U13" s="9">
+      <c r="U13" s="8">
         <v>321</v>
       </c>
-      <c r="V13" s="7">
+      <c r="V13" s="6">
         <v>0.17</v>
       </c>
-      <c r="W13" s="10">
+      <c r="W13" s="9">
         <v>64.48</v>
       </c>
-      <c r="X13" s="10">
+      <c r="X13" s="9">
         <v>47.18</v>
       </c>
-      <c r="Y13" s="10">
+      <c r="Y13" s="9">
         <v>33.159999999999997</v>
       </c>
-      <c r="Z13" s="10">
+      <c r="Z13" s="9">
         <v>28.72</v>
       </c>
-      <c r="AA13" s="10">
+      <c r="AA13" s="9">
         <v>19.98</v>
       </c>
-      <c r="AB13" s="11">
+      <c r="AB13" s="10">
         <v>0.19</v>
       </c>
       <c r="AC13" s="3">
@@ -4199,7 +4369,7 @@
       <c r="AD13" s="3">
         <v>10830</v>
       </c>
-      <c r="AE13" s="12">
+      <c r="AE13" s="11">
         <v>9.09</v>
       </c>
       <c r="AF13" t="s">

</xml_diff>